<commit_message>
Links added to index page
</commit_message>
<xml_diff>
--- a/Media/Content-list-for-Website.xlsx
+++ b/Media/Content-list-for-Website.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noraida Ahmad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prerna_2\github\team-f-project\Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6885"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>https://www.instagram.com/happsters/</t>
   </si>
@@ -183,12 +183,15 @@
   </si>
   <si>
     <t>Update list from time-to-time to remind yourself that life's wonderful!</t>
+  </si>
+  <si>
+    <t>Advice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -249,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,6 +264,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -544,20 +548,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.05078125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -574,7 +578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -582,16 +586,16 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -608,7 +612,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -623,7 +627,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -640,7 +644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -657,7 +661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -674,14 +678,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -698,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>5</v>
       </c>
@@ -715,7 +719,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -732,7 +736,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>5</v>
       </c>
@@ -749,7 +753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>5</v>
       </c>
@@ -766,7 +770,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>5</v>
       </c>
@@ -781,14 +785,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>10</v>
       </c>
@@ -805,7 +809,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>10</v>
       </c>
@@ -822,7 +826,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>10</v>
       </c>
@@ -839,7 +843,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>10</v>
       </c>
@@ -854,7 +858,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>10</v>
       </c>
@@ -869,14 +873,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -886,8 +890,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>